<commit_message>
fixing register and login , cant add two cages with the same number
</commit_message>
<xml_diff>
--- a/ProjectBirdsz/bin/Debug/cages.xlsx
+++ b/ProjectBirdsz/bin/Debug/cages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\Source\Repos\NewBirds\ProjectBirdsz\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16F0566-467D-4EA0-9F63-CDD05503AC50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707B2776-CA5B-46D2-AA9F-7899014015D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11452" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>CageNumber</t>
   </si>
@@ -372,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -506,55 +506,55 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>15</v>
+        <v>223</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>8</v>
+      <c r="A12">
+        <v>12</v>
       </c>
       <c r="B12">
         <v>20</v>
@@ -563,14 +563,48 @@
         <v>35</v>
       </c>
       <c r="D12">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>35</v>
+      </c>
+      <c r="D14">
         <v>80</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fill the birds execl and cages execl only with valid data  ready to push
</commit_message>
<xml_diff>
--- a/ProjectBirdsz/bin/Debug/cages.xlsx
+++ b/ProjectBirdsz/bin/Debug/cages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\Source\Repos\NewBirds\ProjectBirdsz\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{707B2776-CA5B-46D2-AA9F-7899014015D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5298A2CF-401F-4383-8BFD-B312E5948DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11452" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>CageNumber</t>
   </si>
@@ -42,19 +42,13 @@
     <t>Material</t>
   </si>
   <si>
+    <t>Wood</t>
+  </si>
+  <si>
     <t>Plastic</t>
   </si>
   <si>
-    <t>wood</t>
-  </si>
-  <si>
     <t>Metal</t>
-  </si>
-  <si>
-    <t>AAA12</t>
-  </si>
-  <si>
-    <t>Wood</t>
   </si>
 </sst>
 </file>
@@ -372,15 +366,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -397,7 +397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -405,206 +405,85 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D2">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C4">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D4">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C5">
         <v>30</v>
       </c>
       <c r="D5">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>22</v>
-      </c>
-      <c r="C9">
-        <v>223</v>
-      </c>
-      <c r="D9">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>3</v>
-      </c>
-      <c r="C10">
-        <v>15</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11">
-        <v>9</v>
-      </c>
-      <c r="B11">
-        <v>2</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>20</v>
-      </c>
-      <c r="C12">
-        <v>35</v>
-      </c>
-      <c r="D12">
-        <v>48</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14">
-        <v>20</v>
-      </c>
-      <c r="C14">
-        <v>35</v>
-      </c>
-      <c r="D14">
-        <v>80</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E14">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E6">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
sort for the cages , some message box when you fill a wrong number , and we cant add two cages with the same serial numebr
</commit_message>
<xml_diff>
--- a/ProjectBirdsz/bin/Debug/cages.xlsx
+++ b/ProjectBirdsz/bin/Debug/cages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guyal\Source\Repos\NewBirds\ProjectBirdsz\bin\Debug\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3EB4C7-016B-4605-B819-2D601827E76A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D9B600-304B-4566-A3C0-38BAEB3C7B8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
   <si>
     <t>CageNumber</t>
   </si>
@@ -366,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,16 +402,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -533,8 +533,42 @@
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>40</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>30</v>
+      </c>
+      <c r="D11">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>